<commit_message>
Updated: assignment 1 - random integer values.
</commit_message>
<xml_diff>
--- a/OP-2/week-2/assignment/data/assignment_dataset_mod.xlsx
+++ b/OP-2/week-2/assignment/data/assignment_dataset_mod.xlsx
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>72</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3">
@@ -573,7 +573,7 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>39</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4">
@@ -616,7 +616,7 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>72</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5">
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>78</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>88</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7">
@@ -745,7 +745,7 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>72</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8">
@@ -788,7 +788,7 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>8</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9">
@@ -831,7 +831,7 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>52</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10">
@@ -874,7 +874,7 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>84</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11">
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>8</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12">
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>42</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13">
@@ -1003,7 +1003,7 @@
         </is>
       </c>
       <c r="K13" t="n">
-        <v>18</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14">
@@ -1046,7 +1046,7 @@
         </is>
       </c>
       <c r="K14" t="n">
-        <v>40</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15">
@@ -1089,7 +1089,7 @@
         </is>
       </c>
       <c r="K15" t="n">
-        <v>44</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed: usage of wrong df.
</commit_message>
<xml_diff>
--- a/OP-2/week-2/assignment/data/assignment_dataset_mod.xlsx
+++ b/OP-2/week-2/assignment/data/assignment_dataset_mod.xlsx
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>258</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3">
@@ -573,7 +573,7 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>275</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4">
@@ -616,7 +616,7 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>242</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5">
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>138</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>115</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7">
@@ -745,7 +745,7 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>249</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8">
@@ -788,7 +788,7 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>154</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9">
@@ -831,7 +831,7 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>144</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10">
@@ -874,7 +874,7 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>179</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11">
@@ -917,7 +917,7 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>115</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12">
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>186</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13">
@@ -1003,7 +1003,7 @@
         </is>
       </c>
       <c r="K13" t="n">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14">
@@ -1046,7 +1046,7 @@
         </is>
       </c>
       <c r="K14" t="n">
-        <v>132</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15">
@@ -1089,7 +1089,7 @@
         </is>
       </c>
       <c r="K15" t="n">
-        <v>214</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>